<commit_message>
3. hafta ders baslangici
</commit_message>
<xml_diff>
--- a/08_classification/hata_matrisi_precision_recall.xlsx
+++ b/08_classification/hata_matrisi_precision_recall.xlsx
@@ -5,16 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7f10ce1d6aaf8c5d/egitim/verilen/bogazici-compec-python-ml/08_classification/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\egitim\verilen\bogazici-compec-python-ml\08_classification\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E2ADD169-C10B-44EF-B6FD-D562FA568DC0}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2766DF44-E48C-40FB-B5B6-0256F19D4253}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7680" yWindow="1875" windowWidth="15975" windowHeight="11385" xr2:uid="{E430057A-04A5-474B-A4B0-F86040D2C544}"/>
+    <workbookView xWindow="7680" yWindow="1875" windowWidth="15975" windowHeight="13020" xr2:uid="{E430057A-04A5-474B-A4B0-F86040D2C544}"/>
   </bookViews>
   <sheets>
     <sheet name="Sayfa1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sayfa1!$A$1:$C$21</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -25,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="15">
   <si>
     <t>y_test</t>
   </si>
@@ -34,12 +37,53 @@
   </si>
   <si>
     <t>y_pred</t>
+  </si>
+  <si>
+    <t>TP</t>
+  </si>
+  <si>
+    <t>TN</t>
+  </si>
+  <si>
+    <t>FP</t>
+  </si>
+  <si>
+    <t>FN</t>
+  </si>
+  <si>
+    <t>Accuracy</t>
+  </si>
+  <si>
+    <t>Precision</t>
+  </si>
+  <si>
+    <t>Recall</t>
+  </si>
+  <si>
+    <t>Eşik: 0.5</t>
+  </si>
+  <si>
+    <t>Eşik: 0.3</t>
+  </si>
+  <si>
+    <t>Eşik: 0.7</t>
+  </si>
+  <si>
+    <t>Mümkün olduğunca 
+gerçek sınıfı bilme</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hata yapmayalım 
+Yanlışa doğru demeyelim </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -70,10 +114,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -389,10 +440,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E535F0B3-D41F-445F-A34F-DD8FA473BF5E}">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:K38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A21"/>
+      <selection activeCell="M27" sqref="M27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -424,7 +475,7 @@
         <v>0</v>
       </c>
       <c r="B3">
-        <v>0.32100000000000001</v>
+        <v>0.22900000000000001</v>
       </c>
       <c r="C3" s="1">
         <v>0</v>
@@ -457,7 +508,7 @@
         <v>0</v>
       </c>
       <c r="B6">
-        <v>0.432</v>
+        <v>0.45700000000000002</v>
       </c>
       <c r="C6" s="1">
         <v>0</v>
@@ -468,7 +519,7 @@
         <v>0</v>
       </c>
       <c r="B7">
-        <v>0.45700000000000002</v>
+        <v>0.47799999999999998</v>
       </c>
       <c r="C7" s="1">
         <v>0</v>
@@ -476,10 +527,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B8">
-        <v>0.47799999999999998</v>
+        <v>0.48099999999999998</v>
       </c>
       <c r="C8" s="1">
         <v>0</v>
@@ -490,7 +541,7 @@
         <v>0</v>
       </c>
       <c r="B9">
-        <v>0.48</v>
+        <v>0.48799999999999999</v>
       </c>
       <c r="C9" s="1">
         <v>0</v>
@@ -501,7 +552,7 @@
         <v>0</v>
       </c>
       <c r="B10">
-        <v>0.48799999999999999</v>
+        <v>0.49299999999999999</v>
       </c>
       <c r="C10" s="1">
         <v>0</v>
@@ -509,10 +560,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B11">
-        <v>0.49299999999999999</v>
+        <v>0.52900000000000003</v>
       </c>
       <c r="C11" s="1">
         <v>0</v>
@@ -520,24 +571,24 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B12">
-        <v>0.52900000000000003</v>
+        <v>0.55300000000000005</v>
       </c>
       <c r="C12" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B13">
-        <v>0.55300000000000005</v>
+        <v>0.63200000000000001</v>
       </c>
       <c r="C13" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -548,7 +599,7 @@
         <v>0.67200000000000004</v>
       </c>
       <c r="C14" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -573,7 +624,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>1</v>
       </c>
@@ -584,7 +635,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>1</v>
       </c>
@@ -595,7 +646,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>1</v>
       </c>
@@ -606,7 +657,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>1</v>
       </c>
@@ -617,7 +668,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>1</v>
       </c>
@@ -628,7 +679,203 @@
         <v>1</v>
       </c>
     </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" t="s">
+        <v>10</v>
+      </c>
+      <c r="G23" t="s">
+        <v>11</v>
+      </c>
+      <c r="J23" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D24" t="s">
+        <v>3</v>
+      </c>
+      <c r="E24">
+        <v>9</v>
+      </c>
+      <c r="G24" t="s">
+        <v>3</v>
+      </c>
+      <c r="H24">
+        <v>10</v>
+      </c>
+      <c r="J24" t="s">
+        <v>3</v>
+      </c>
+      <c r="K24">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D25" t="s">
+        <v>4</v>
+      </c>
+      <c r="E25">
+        <v>8</v>
+      </c>
+      <c r="G25" t="s">
+        <v>4</v>
+      </c>
+      <c r="H25">
+        <v>2</v>
+      </c>
+      <c r="J25" t="s">
+        <v>4</v>
+      </c>
+      <c r="K25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D26" t="s">
+        <v>5</v>
+      </c>
+      <c r="E26">
+        <v>2</v>
+      </c>
+      <c r="G26" t="s">
+        <v>5</v>
+      </c>
+      <c r="H26">
+        <v>8</v>
+      </c>
+      <c r="J26" t="s">
+        <v>5</v>
+      </c>
+      <c r="K26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D27" t="s">
+        <v>6</v>
+      </c>
+      <c r="E27">
+        <v>1</v>
+      </c>
+      <c r="G27" t="s">
+        <v>6</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+      <c r="J27" t="s">
+        <v>6</v>
+      </c>
+      <c r="K27">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D28" t="s">
+        <v>7</v>
+      </c>
+      <c r="E28" s="2">
+        <f>((E24+E25) / SUM(E24:E27))</f>
+        <v>0.85</v>
+      </c>
+      <c r="G28" t="s">
+        <v>7</v>
+      </c>
+      <c r="H28" s="2">
+        <f>((H24+H25) / SUM(H24:H27))</f>
+        <v>0.6</v>
+      </c>
+      <c r="J28" t="s">
+        <v>7</v>
+      </c>
+      <c r="K28" s="2">
+        <f>((K24+K25) / SUM(K24:K27))</f>
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D29" t="s">
+        <v>8</v>
+      </c>
+      <c r="E29" s="2">
+        <f>((E24) / (E24+E26))</f>
+        <v>0.81818181818181823</v>
+      </c>
+      <c r="G29" t="s">
+        <v>8</v>
+      </c>
+      <c r="H29" s="2">
+        <f>((H24) / (H24+H26))</f>
+        <v>0.55555555555555558</v>
+      </c>
+      <c r="J29" t="s">
+        <v>8</v>
+      </c>
+      <c r="K29" s="2">
+        <f>((K24) / (K24+K26))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D30" t="s">
+        <v>9</v>
+      </c>
+      <c r="E30" s="2">
+        <f>((E24) / (E24 + E27))</f>
+        <v>0.9</v>
+      </c>
+      <c r="G30" t="s">
+        <v>9</v>
+      </c>
+      <c r="H30" s="2">
+        <f>((H24) / (H24 + H27))</f>
+        <v>1</v>
+      </c>
+      <c r="J30" t="s">
+        <v>9</v>
+      </c>
+      <c r="K30" s="2">
+        <f>((K24) / (K24 + K27))</f>
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="33" spans="4:11" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+      <c r="G33" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H33" s="4"/>
+      <c r="J33" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K33" s="3"/>
+    </row>
+    <row r="35" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="E35" s="2"/>
+    </row>
+    <row r="36" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="E36" s="2"/>
+    </row>
+    <row r="37" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="E37" s="2"/>
+    </row>
+    <row r="38" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="E38" s="2"/>
+    </row>
   </sheetData>
+  <autoFilter ref="A1:C21" xr:uid="{C42D783A-7CE6-490C-AFED-76A7CDA8840B}"/>
+  <sortState ref="A2:E30">
+    <sortCondition ref="B3"/>
+  </sortState>
+  <mergeCells count="3">
+    <mergeCell ref="G33:H33"/>
+    <mergeCell ref="J33:K33"/>
+    <mergeCell ref="D33:E33"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>